<commit_message>
Summer - Tuna Salad with apple and celery
</commit_message>
<xml_diff>
--- a/data/TunaSaladWithAppleAndCelerySummer.xlsx
+++ b/data/TunaSaladWithAppleAndCelerySummer.xlsx
@@ -8,14 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\denis\eclipse-workspace\wildfit-ETL\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B8C6737-60FA-4D8E-A5A9-F5C1F6632AFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3D6AEC7-CD9E-4980-8794-B330C458C7AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="3645" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="360" yWindow="3645" windowWidth="22500" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Dressing" sheetId="3" r:id="rId2"/>
-    <sheet name="Salad" sheetId="2" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,15 +26,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="53">
   <si>
     <t>Season</t>
   </si>
   <si>
     <t>Title</t>
-  </si>
-  <si>
-    <t>summer</t>
   </si>
   <si>
     <t>Tuna salad with apple and celery (Summer)</t>
@@ -103,21 +99,12 @@
     <t>can</t>
   </si>
   <si>
-    <t>foodName</t>
-  </si>
-  <si>
-    <t>real mayonnaise, sugar-free</t>
-  </si>
-  <si>
     <t>1 tbsp sugar-free mayonnaise</t>
   </si>
   <si>
     <t>tbsp</t>
   </si>
   <si>
-    <t>Greek Yoghurt, Plain</t>
-  </si>
-  <si>
     <t>1 tbsp Greek yoghurt</t>
   </si>
   <si>
@@ -182,6 +169,24 @@
   </si>
   <si>
     <t>4 cornichon (small sugar free pickled cucumbers)</t>
+  </si>
+  <si>
+    <t>Dressing</t>
+  </si>
+  <si>
+    <t>Salad</t>
+  </si>
+  <si>
+    <t>Food</t>
+  </si>
+  <si>
+    <t>plain Greek yogurt</t>
+  </si>
+  <si>
+    <t>sugar-free mayonnaise</t>
+  </si>
+  <si>
+    <t>SUMMER</t>
   </si>
 </sst>
 </file>
@@ -513,13 +518,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="40" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="88.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.28515625" bestFit="1" customWidth="1"/>
@@ -536,30 +541,30 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
       <c r="C2" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D2">
         <v>15</v>
@@ -571,7 +576,7 @@
         <v>4</v>
       </c>
       <c r="G2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -581,323 +586,287 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB6C9362-A1F8-463F-82B5-4B4DB195D565}">
-  <dimension ref="A1:H5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D72576DC-2686-4A61-B487-4806851E93F0}">
+  <dimension ref="A1:I17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="48.28515625" customWidth="1"/>
-    <col min="6" max="6" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="71.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="46.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>4</v>
+      </c>
+      <c r="C6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7" t="s">
+        <v>33</v>
+      </c>
+      <c r="F7" t="s">
+        <v>21</v>
+      </c>
+      <c r="G7">
+        <v>2</v>
+      </c>
+      <c r="H7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D8">
+        <v>2</v>
+      </c>
+      <c r="E8" t="s">
+        <v>34</v>
+      </c>
+      <c r="F8" t="s">
+        <v>35</v>
+      </c>
+      <c r="G8">
+        <v>0.5</v>
+      </c>
+      <c r="H8" t="s">
+        <v>34</v>
+      </c>
+      <c r="I8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D9">
+        <v>3</v>
+      </c>
+      <c r="E9" t="s">
+        <v>37</v>
+      </c>
+      <c r="F9" t="s">
+        <v>38</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+      <c r="H9" t="s">
+        <v>39</v>
+      </c>
+      <c r="I9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D10">
+        <v>4</v>
+      </c>
+      <c r="E10" t="s">
+        <v>40</v>
+      </c>
+      <c r="F10" t="s">
+        <v>41</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="H10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D11">
         <v>5</v>
       </c>
-      <c r="B1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="E11" t="s">
+        <v>42</v>
+      </c>
+      <c r="F11" t="s">
+        <v>43</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+      <c r="H11" t="s">
+        <v>44</v>
+      </c>
+      <c r="I11" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D12">
+        <v>6</v>
+      </c>
+      <c r="E12" t="s">
+        <v>45</v>
+      </c>
+      <c r="F12" t="s">
+        <v>46</v>
+      </c>
+      <c r="G12">
+        <v>4</v>
+      </c>
+      <c r="H12" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14" t="s">
+        <v>51</v>
+      </c>
+      <c r="F14" t="s">
+        <v>23</v>
+      </c>
+      <c r="G14">
+        <v>1</v>
+      </c>
+      <c r="H14" t="s">
         <v>24</v>
       </c>
-      <c r="E1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G1" t="s">
-        <v>20</v>
-      </c>
-      <c r="H1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2" t="s">
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D15">
+        <v>2</v>
+      </c>
+      <c r="E15" t="s">
+        <v>50</v>
+      </c>
+      <c r="F15" t="s">
         <v>25</v>
       </c>
-      <c r="E2" t="s">
+      <c r="G15">
+        <v>1</v>
+      </c>
+      <c r="H15" t="s">
+        <v>24</v>
+      </c>
+      <c r="I15" t="s">
         <v>26</v>
       </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-      <c r="G2" t="s">
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D16">
+        <v>3</v>
+      </c>
+      <c r="E16" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C3">
-        <v>2</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="F16" t="s">
         <v>28</v>
       </c>
-      <c r="E3" t="s">
+      <c r="G16">
+        <v>0.125</v>
+      </c>
+      <c r="H16" t="s">
         <v>29</v>
       </c>
-      <c r="F3">
-        <v>1</v>
-      </c>
-      <c r="G3" t="s">
-        <v>27</v>
-      </c>
-      <c r="H3" t="s">
+      <c r="I16" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C4">
-        <v>3</v>
-      </c>
-      <c r="D4" t="s">
+    <row r="17" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D17">
+        <v>4</v>
+      </c>
+      <c r="E17" t="s">
         <v>31</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F17" t="s">
         <v>32</v>
       </c>
-      <c r="F4">
+      <c r="G17">
         <v>0.125</v>
       </c>
-      <c r="G4" t="s">
-        <v>33</v>
-      </c>
-      <c r="H4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C5">
-        <v>4</v>
-      </c>
-      <c r="D5" t="s">
-        <v>35</v>
-      </c>
-      <c r="E5" t="s">
-        <v>36</v>
-      </c>
-      <c r="F5">
-        <v>0.125</v>
-      </c>
-      <c r="G5" t="s">
-        <v>33</v>
-      </c>
-      <c r="H5" t="s">
-        <v>34</v>
+      <c r="H17" t="s">
+        <v>29</v>
+      </c>
+      <c r="I17" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D72576DC-2686-4A61-B487-4806851E93F0}">
-  <dimension ref="A1:H11"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:H1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="71.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="46.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G1" t="s">
-        <v>20</v>
-      </c>
-      <c r="H1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C6">
-        <v>1</v>
-      </c>
-      <c r="D6" t="s">
-        <v>37</v>
-      </c>
-      <c r="E6" t="s">
-        <v>22</v>
-      </c>
-      <c r="F6">
-        <v>2</v>
-      </c>
-      <c r="G6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C7">
-        <v>2</v>
-      </c>
-      <c r="D7" t="s">
-        <v>38</v>
-      </c>
-      <c r="E7" t="s">
-        <v>39</v>
-      </c>
-      <c r="F7">
-        <v>0.5</v>
-      </c>
-      <c r="G7" t="s">
-        <v>38</v>
-      </c>
-      <c r="H7" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C8">
-        <v>3</v>
-      </c>
-      <c r="D8" t="s">
-        <v>41</v>
-      </c>
-      <c r="E8" t="s">
-        <v>42</v>
-      </c>
-      <c r="F8">
-        <v>1</v>
-      </c>
-      <c r="G8" t="s">
-        <v>43</v>
-      </c>
-      <c r="H8" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C9">
-        <v>4</v>
-      </c>
-      <c r="D9" t="s">
-        <v>44</v>
-      </c>
-      <c r="E9" t="s">
-        <v>45</v>
-      </c>
-      <c r="F9">
-        <v>1</v>
-      </c>
-      <c r="G9" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C10">
-        <v>5</v>
-      </c>
-      <c r="D10" t="s">
-        <v>46</v>
-      </c>
-      <c r="E10" t="s">
-        <v>47</v>
-      </c>
-      <c r="F10">
-        <v>1</v>
-      </c>
-      <c r="G10" t="s">
-        <v>48</v>
-      </c>
-      <c r="H10" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C11">
-        <v>6</v>
-      </c>
-      <c r="D11" t="s">
-        <v>49</v>
-      </c>
-      <c r="E11" t="s">
-        <v>50</v>
-      </c>
-      <c r="F11">
-        <v>4</v>
-      </c>
-      <c r="G11" t="s">
-        <v>49</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>